<commit_message>
Added note about 2020 brackets, no nubs
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie BOM.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie BOM.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="859" documentId="13_ncr:40009_{88348E9D-FB72-456D-96C4-609C2DEF09D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7E2A21B-D366-43B5-A910-3305D811AB24}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Valkyrie Base Frame BOM 02" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Valkyrie Base Frame BOM 02'!$A$11:$P$55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Valkyrie Base Frame BOM 02'!$A$1:$P$57</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Roy Berntsen</author>
   </authors>
   <commentList>
-    <comment ref="D34" authorId="0" shapeId="0" xr:uid="{FB4E5E39-3716-46C1-9030-8ED6146980D7}">
+    <comment ref="D34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0" shapeId="0" xr:uid="{F7999DE5-A231-4BE3-8A97-2FA9AF556EFC}">
+    <comment ref="D41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -113,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="135">
   <si>
     <t>PROJECT VALKYRIE</t>
   </si>
@@ -515,19 +509,22 @@
   </si>
   <si>
     <t>Length: 60mm 3PC</t>
+  </si>
+  <si>
+    <t>smooth back, no nubs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.0_ ;_-[$$-409]* \-#,##0.0\ ;_-[$$-409]* &quot;-&quot;?_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1376,7 +1373,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A14C330-9941-4B9D-BB36-3276622CD721}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4A14C330-9941-4B9D-BB36-3276622CD721}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1699,24 +1696,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P57"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1735,7 +1732,7 @@
     <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="26.25">
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
@@ -1755,7 +1752,7 @@
       <c r="O1" s="47"/>
       <c r="P1" s="47"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="48"/>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -1773,40 +1770,40 @@
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:16" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15.75" thickBot="1"/>
+    <row r="11" spans="1:16" s="7" customFormat="1" ht="30.75" thickBot="1">
       <c r="A11" s="17" t="s">
         <v>5</v>
       </c>
@@ -1856,7 +1853,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" s="26" t="s">
         <v>17</v>
       </c>
@@ -1889,7 +1886,7 @@
       <c r="O12" s="27"/>
       <c r="P12" s="31"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1922,7 +1919,7 @@
       <c r="O13" s="32"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1955,7 +1952,7 @@
       <c r="O14" s="32"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1988,7 +1985,7 @@
       <c r="O15" s="32"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
@@ -2032,7 +2029,7 @@
       <c r="O16" s="8"/>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -2076,7 +2073,7 @@
       <c r="O17" s="32"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
@@ -2114,7 +2111,7 @@
       <c r="O18" s="23"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2151,8 +2148,11 @@
       <c r="N19" s="35"/>
       <c r="O19" s="32"/>
       <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -2190,7 +2190,7 @@
       <c r="O20" s="32"/>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2234,7 +2234,7 @@
       <c r="O21" s="32"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -2276,7 +2276,7 @@
       <c r="O22" s="32"/>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -2318,7 +2318,7 @@
       <c r="O23" s="32"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
@@ -2360,7 +2360,7 @@
       <c r="O24" s="32"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="O25" s="32"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -2442,7 +2442,7 @@
       <c r="O26" s="32"/>
       <c r="P26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="O27" s="32"/>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -2519,7 +2519,7 @@
       <c r="O28" s="32"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
@@ -2555,7 +2555,7 @@
       <c r="O29" s="32"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
@@ -2591,7 +2591,7 @@
       <c r="O30" s="32"/>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -2627,7 +2627,7 @@
       <c r="O31" s="32"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>7380</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" s="2" t="s">
         <v>41</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="O33" s="32"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -2741,7 +2741,7 @@
       <c r="O34" s="32"/>
       <c r="P34" s="3"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" s="2" t="s">
         <v>41</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="O35" s="32"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -2817,7 +2817,7 @@
       <c r="O36" s="32"/>
       <c r="P36" s="3"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -2855,7 +2855,7 @@
       <c r="O37" s="32"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
@@ -2899,7 +2899,7 @@
       <c r="O38" s="32"/>
       <c r="P38" s="3"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -2930,7 +2930,7 @@
       <c r="O39" s="32"/>
       <c r="P39" s="3"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
@@ -2961,7 +2961,7 @@
       <c r="O40" s="32"/>
       <c r="P40" s="3"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" s="2" t="s">
         <v>108</v>
       </c>
@@ -2999,7 +2999,7 @@
       <c r="O41" s="32"/>
       <c r="P41" s="3"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" s="2" t="s">
         <v>108</v>
       </c>
@@ -3037,7 +3037,7 @@
       <c r="O42" s="32"/>
       <c r="P42" s="3"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" s="2" t="s">
         <v>113</v>
       </c>
@@ -3075,7 +3075,7 @@
       <c r="O43" s="32"/>
       <c r="P43" s="3"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="A44" s="2" t="s">
         <v>113</v>
       </c>
@@ -3113,7 +3113,7 @@
       <c r="O44" s="32"/>
       <c r="P44" s="3"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
@@ -3153,7 +3153,7 @@
       <c r="O45" s="32"/>
       <c r="P45" s="3"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
@@ -3195,7 +3195,7 @@
       <c r="O46" s="32"/>
       <c r="P46" s="3"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -3237,7 +3237,7 @@
       <c r="O47" s="32"/>
       <c r="P47" s="3"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16">
       <c r="A48" s="2" t="s">
         <v>45</v>
       </c>
@@ -3279,7 +3279,7 @@
       <c r="O48" s="32"/>
       <c r="P48" s="3"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="A49" s="2" t="s">
         <v>45</v>
       </c>
@@ -3318,7 +3318,7 @@
       <c r="O49" s="32"/>
       <c r="P49" s="3"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="A50" s="2" t="s">
         <v>45</v>
       </c>
@@ -3358,7 +3358,7 @@
       <c r="O50" s="32"/>
       <c r="P50" s="3"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16">
       <c r="A51" s="2" t="s">
         <v>45</v>
       </c>
@@ -3398,7 +3398,7 @@
       <c r="O51" s="32"/>
       <c r="P51" s="3"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16">
       <c r="A52" s="2" t="s">
         <v>81</v>
       </c>
@@ -3426,7 +3426,7 @@
       <c r="O52" s="32"/>
       <c r="P52" s="3"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="A53" s="2" t="s">
         <v>81</v>
       </c>
@@ -3454,7 +3454,7 @@
       <c r="O53" s="32"/>
       <c r="P53" s="3"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16">
       <c r="A54" s="2" t="s">
         <v>81</v>
       </c>
@@ -3480,7 +3480,7 @@
       <c r="O54" s="32"/>
       <c r="P54" s="3"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="A55" s="2" t="s">
         <v>81</v>
       </c>
@@ -3506,7 +3506,7 @@
       <c r="O55" s="32"/>
       <c r="P55" s="3"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="A56" s="2"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
@@ -3524,7 +3524,7 @@
       <c r="O56" s="32"/>
       <c r="P56" s="3"/>
     </row>
-    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="15.75" thickBot="1">
       <c r="A57" s="4" t="s">
         <v>51</v>
       </c>
@@ -3552,40 +3552,40 @@
       <c r="P57" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:P55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A11:P55"/>
   <mergeCells count="2">
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K45" r:id="rId1" xr:uid="{AA6174A7-7F32-4CA5-815C-1D533DDE9F41}"/>
-    <hyperlink ref="K46" r:id="rId2" display="Link" xr:uid="{3534C385-06DC-4CA4-9BD2-43314754659B}"/>
-    <hyperlink ref="K47" r:id="rId3" display="Link" xr:uid="{182FB9B2-97AA-4C37-B920-E3964DCD972B}"/>
-    <hyperlink ref="K48" r:id="rId4" display="Link" xr:uid="{F71A0265-955D-4D26-B211-E32D15EE1D56}"/>
-    <hyperlink ref="K49" r:id="rId5" display="Link" xr:uid="{B9C35A18-9E24-41B8-8C22-68FEA326621C}"/>
-    <hyperlink ref="N50" r:id="rId6" display="Compact Powerful Motor" xr:uid="{9EFF2727-C3AB-4597-8B26-0F812CAFC429}"/>
-    <hyperlink ref="N51" r:id="rId7" xr:uid="{605BE8D7-BA93-4401-9D46-9E08E1D04442}"/>
-    <hyperlink ref="K21" r:id="rId8" display="Link" xr:uid="{695B4940-C0A7-4809-BDF2-0C233AA6AE26}"/>
-    <hyperlink ref="K23" r:id="rId9" display="2x Length: 45mm 4PC" xr:uid="{6B68950A-869F-4FCE-BC1C-F219E055C5B9}"/>
-    <hyperlink ref="K33" r:id="rId10" xr:uid="{24787D90-0D34-481E-9743-F212E75A3881}"/>
-    <hyperlink ref="K25" r:id="rId11" xr:uid="{D6A1DF84-384D-40FB-BD4A-701A0F364D79}"/>
-    <hyperlink ref="N46" r:id="rId12" display="Gates" xr:uid="{E093F5B4-8BAD-4356-A43B-07E9B513EAC3}"/>
-    <hyperlink ref="N47" r:id="rId13" display="Gates" xr:uid="{49D5B23E-126C-4370-A262-C5184F11CAFE}"/>
-    <hyperlink ref="N48" r:id="rId14" display="Pulley 20 Tooth 9mm" xr:uid="{27F936CE-C292-435B-B7DE-316A6986F2BD}"/>
-    <hyperlink ref="K26" r:id="rId15" xr:uid="{A8C5E0F3-B1FB-4E57-8DD8-1DF57CDC1A28}"/>
-    <hyperlink ref="K35" r:id="rId16" xr:uid="{ACB41F0C-D739-4C4C-B9A7-3FBBB0E03C0B}"/>
-    <hyperlink ref="K34" r:id="rId17" display="FYSETC Big Dipper" xr:uid="{531DCC85-6FB5-4C6C-8657-8A481CD30069}"/>
-    <hyperlink ref="K36" r:id="rId18" display="6pcs Optical Endstop" xr:uid="{0AB90FFF-9946-4F78-93E2-A102C645ECAE}"/>
-    <hyperlink ref="K37" r:id="rId19" xr:uid="{1A2B703D-766E-449D-AD03-BDC8990C9635}"/>
-    <hyperlink ref="K22" r:id="rId20" xr:uid="{7E1F7424-E58C-4FCB-9D3A-3CB69F34CE9F}"/>
-    <hyperlink ref="K27" r:id="rId21" xr:uid="{755FCD6D-D745-447C-AAA6-2D31A19F9A40}"/>
-    <hyperlink ref="K41" r:id="rId22" xr:uid="{A90E869A-7328-473A-BA20-82979A845F00}"/>
-    <hyperlink ref="K42" r:id="rId23" xr:uid="{37B2932B-CA7B-49AA-9F35-9BCE3D136353}"/>
-    <hyperlink ref="K43" r:id="rId24" xr:uid="{BE140B59-D4B8-46C3-B6EC-BEB5F431781F}"/>
-    <hyperlink ref="K44" r:id="rId25" xr:uid="{54817A0E-3A4B-42D7-AA92-5C84B2F161F2}"/>
-    <hyperlink ref="K38" r:id="rId26" xr:uid="{4F053E16-31A4-458E-B422-7E74FE54E665}"/>
-    <hyperlink ref="N38" r:id="rId27" display="Color: 220V 750W" xr:uid="{6A46011B-C1CA-4A88-AD58-75064F9710C4}"/>
-    <hyperlink ref="K24" r:id="rId28" xr:uid="{D81B7FCC-2A0B-49BE-B9F6-1DF3B108016A}"/>
+    <hyperlink ref="K45" r:id="rId1"/>
+    <hyperlink ref="K46" r:id="rId2" display="Link"/>
+    <hyperlink ref="K47" r:id="rId3" display="Link"/>
+    <hyperlink ref="K48" r:id="rId4" display="Link"/>
+    <hyperlink ref="K49" r:id="rId5" display="Link"/>
+    <hyperlink ref="N50" r:id="rId6" display="Compact Powerful Motor"/>
+    <hyperlink ref="N51" r:id="rId7"/>
+    <hyperlink ref="K21" r:id="rId8" display="Link"/>
+    <hyperlink ref="K23" r:id="rId9" display="2x Length: 45mm 4PC"/>
+    <hyperlink ref="K33" r:id="rId10"/>
+    <hyperlink ref="K25" r:id="rId11"/>
+    <hyperlink ref="N46" r:id="rId12" display="Gates"/>
+    <hyperlink ref="N47" r:id="rId13" display="Gates"/>
+    <hyperlink ref="N48" r:id="rId14" display="Pulley 20 Tooth 9mm"/>
+    <hyperlink ref="K26" r:id="rId15"/>
+    <hyperlink ref="K35" r:id="rId16"/>
+    <hyperlink ref="K34" r:id="rId17" display="FYSETC Big Dipper"/>
+    <hyperlink ref="K36" r:id="rId18" display="6pcs Optical Endstop"/>
+    <hyperlink ref="K37" r:id="rId19"/>
+    <hyperlink ref="K22" r:id="rId20"/>
+    <hyperlink ref="K27" r:id="rId21"/>
+    <hyperlink ref="K41" r:id="rId22"/>
+    <hyperlink ref="K42" r:id="rId23"/>
+    <hyperlink ref="K43" r:id="rId24"/>
+    <hyperlink ref="K44" r:id="rId25"/>
+    <hyperlink ref="K38" r:id="rId26"/>
+    <hyperlink ref="N38" r:id="rId27" display="Color: 220V 750W"/>
+    <hyperlink ref="K24" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId29"/>

</xml_diff>

<commit_message>
ab 7 lab update
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie BOM.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="860" documentId="13_ncr:40009_{88348E9D-FB72-456D-96C4-609C2DEF09D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{146FF297-362F-4734-B3CE-4DD5A49D2953}"/>
+  <xr:revisionPtr revIDLastSave="876" documentId="13_ncr:40009_{88348E9D-FB72-456D-96C4-609C2DEF09D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{850D29E6-7F83-4808-A3EA-931A2DFC41ED}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Valkyrie Base Frame BOM 02" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Valkyrie Base Frame BOM 02'!$A$11:$P$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Valkyrie Base Frame BOM 02'!$A$10:$P$55</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Valkyrie Base Frame BOM 02'!$A$1:$P$57</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="136">
   <si>
     <t>PROJECT VALKYRIE</t>
   </si>
@@ -515,6 +515,12 @@
   </si>
   <si>
     <t>Length: 60mm 3PC</t>
+  </si>
+  <si>
+    <t>D5xL55 M4 Shoulder Screw</t>
+  </si>
+  <si>
+    <t>M4-D5mm - 55mm</t>
   </si>
 </sst>
 </file>
@@ -1360,16 +1366,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>476248</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161328</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1397,8 +1403,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5391151" y="352425"/>
-          <a:ext cx="2962272" cy="1666278"/>
+          <a:off x="5324476" y="352425"/>
+          <a:ext cx="2514599" cy="1414462"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1805,109 +1811,142 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:16" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:16" s="7" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B10" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F10" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H10" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I10" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J10" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="K11" s="19" t="s">
+      <c r="K10" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="M11" s="18" t="s">
+      <c r="M10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="O11" s="18" t="s">
+      <c r="O10" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="P11" s="19" t="s">
+      <c r="P10" s="19" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="27">
+        <v>500</v>
+      </c>
+      <c r="F11" s="28">
+        <f>G11*E11</f>
+        <v>500</v>
+      </c>
+      <c r="G11" s="28">
+        <v>1</v>
+      </c>
+      <c r="H11" s="28"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="31"/>
+    </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="27">
-        <v>500</v>
-      </c>
-      <c r="F12" s="28">
+      <c r="C12" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="32">
+        <v>420</v>
+      </c>
+      <c r="F12" s="33">
         <f>G12*E12</f>
-        <v>500</v>
-      </c>
-      <c r="G12" s="28">
-        <v>1</v>
-      </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="31"/>
+        <v>1680</v>
+      </c>
+      <c r="G12" s="33">
+        <v>4</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="45" t="s">
         <v>129</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="32">
-        <v>420</v>
+        <v>460</v>
       </c>
       <c r="F13" s="33">
-        <f>G13*E13</f>
-        <v>1680</v>
+        <f t="shared" ref="F13:F14" si="0">G13*E13</f>
+        <v>1840</v>
       </c>
       <c r="G13" s="33">
         <v>4</v>
@@ -1933,14 +1972,14 @@
         <v>20</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E14" s="32">
-        <v>460</v>
+        <v>700</v>
       </c>
       <c r="F14" s="33">
-        <f t="shared" ref="F14:F15" si="0">G14*E14</f>
-        <v>1840</v>
+        <f t="shared" si="0"/>
+        <v>2800</v>
       </c>
       <c r="G14" s="33">
         <v>4</v>
@@ -1956,163 +1995,168 @@
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1500</v>
+      </c>
+      <c r="F15" s="20">
+        <f>F12+F13+F14</f>
+        <v>6320</v>
+      </c>
+      <c r="G15" s="21">
+        <f>F15/E15</f>
+        <v>4.2133333333333329</v>
+      </c>
+      <c r="H15" s="22">
+        <v>5</v>
+      </c>
+      <c r="I15" s="13">
+        <v>23.2</v>
+      </c>
+      <c r="J15" s="15">
+        <f>H15*I15</f>
+        <v>116</v>
+      </c>
+      <c r="K15" s="40"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="35">
+        <f t="shared" ref="M15:M45" si="1">L15*H15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="15"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="32">
+        <v>500</v>
+      </c>
+      <c r="F16" s="36">
+        <f>F11</f>
+        <v>500</v>
+      </c>
+      <c r="G16" s="32">
+        <f>F16/E16</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="37">
+        <v>1</v>
+      </c>
+      <c r="I16" s="34">
+        <v>6</v>
+      </c>
+      <c r="J16" s="35">
+        <f>H16*I16</f>
+        <v>6</v>
+      </c>
+      <c r="K16" s="41"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N16" s="35"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="32">
-        <v>700</v>
-      </c>
-      <c r="F15" s="33">
-        <f t="shared" si="0"/>
-        <v>2800</v>
-      </c>
-      <c r="G15" s="33">
-        <v>4</v>
-      </c>
-      <c r="H15" s="33"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="3"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="D17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24">
+        <v>12</v>
+      </c>
+      <c r="H17" s="24">
+        <v>12</v>
+      </c>
+      <c r="I17" s="14">
+        <v>2</v>
+      </c>
+      <c r="J17" s="16">
+        <f>H17*I17</f>
         <v>24</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="8">
-        <v>1500</v>
-      </c>
-      <c r="F16" s="20">
-        <f>F13+F14+F15</f>
-        <v>6320</v>
-      </c>
-      <c r="G16" s="21">
-        <f>F16/E16</f>
-        <v>4.2133333333333329</v>
-      </c>
-      <c r="H16" s="22">
-        <v>5</v>
-      </c>
-      <c r="I16" s="13">
-        <v>23.2</v>
-      </c>
-      <c r="J16" s="15">
-        <f>H16*I16</f>
-        <v>116</v>
-      </c>
-      <c r="K16" s="40"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="35">
-        <f t="shared" ref="M16:M45" si="1">L16*H16</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="15"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="32">
-        <v>500</v>
-      </c>
-      <c r="F17" s="36">
-        <f>F12</f>
-        <v>500</v>
-      </c>
-      <c r="G17" s="32">
-        <f>F17/E17</f>
-        <v>1</v>
-      </c>
-      <c r="H17" s="37">
-        <v>1</v>
-      </c>
-      <c r="I17" s="34">
-        <v>6</v>
-      </c>
-      <c r="J17" s="35">
-        <f>H17*I17</f>
-        <v>6</v>
-      </c>
-      <c r="K17" s="41"/>
-      <c r="L17" s="35"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="16"/>
       <c r="M17" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N17" s="35"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="3"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="12"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="C18" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24">
-        <v>12</v>
-      </c>
-      <c r="H18" s="24">
-        <v>12</v>
-      </c>
-      <c r="I18" s="14">
-        <v>2</v>
-      </c>
-      <c r="J18" s="16">
+      <c r="C18" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33">
+        <v>6</v>
+      </c>
+      <c r="H18" s="33">
+        <v>10</v>
+      </c>
+      <c r="I18" s="38">
+        <v>0.8</v>
+      </c>
+      <c r="J18" s="35">
         <f>H18*I18</f>
-        <v>24</v>
-      </c>
-      <c r="K18" s="12"/>
-      <c r="L18" s="16"/>
+        <v>8</v>
+      </c>
+      <c r="K18" s="42"/>
+      <c r="L18" s="35"/>
       <c r="M18" s="35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="16"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="12"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="3"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
@@ -2125,24 +2169,24 @@
         <v>29</v>
       </c>
       <c r="D19" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="33"/>
       <c r="G19" s="33">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="H19" s="33">
-        <v>10</v>
-      </c>
-      <c r="I19" s="38">
-        <v>0.8</v>
+        <v>32</v>
+      </c>
+      <c r="I19" s="34">
+        <v>1.03</v>
       </c>
       <c r="J19" s="35">
-        <f>H19*I19</f>
-        <v>8</v>
-      </c>
-      <c r="K19" s="42"/>
+        <f t="shared" ref="J19:J51" si="2">H19*I19</f>
+        <v>32.96</v>
+      </c>
+      <c r="K19" s="3"/>
       <c r="L19" s="35"/>
       <c r="M19" s="35">
         <f t="shared" si="1"/>
@@ -2160,27 +2204,33 @@
         <v>129</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D20" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
+        <v>33</v>
+      </c>
+      <c r="E20" s="32">
+        <v>410</v>
+      </c>
+      <c r="F20" s="33">
+        <v>500</v>
+      </c>
       <c r="G20" s="33">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="H20" s="33">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="I20" s="34">
-        <v>1.03</v>
+        <v>20</v>
       </c>
       <c r="J20" s="35">
-        <f t="shared" ref="J20:J51" si="2">H20*I20</f>
-        <v>32.96</v>
-      </c>
-      <c r="K20" s="3"/>
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="K20" s="43" t="s">
+        <v>69</v>
+      </c>
       <c r="L20" s="35"/>
       <c r="M20" s="35">
         <f t="shared" si="1"/>
@@ -2195,35 +2245,33 @@
         <v>17</v>
       </c>
       <c r="B21" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>33</v>
+        <v>130</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>60</v>
       </c>
       <c r="E21" s="32">
-        <v>410</v>
-      </c>
-      <c r="F21" s="33">
-        <v>500</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F21" s="33"/>
       <c r="G21" s="33">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H21" s="33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I21" s="34">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="J21" s="35">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="K21" s="43" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="L21" s="35"/>
       <c r="M21" s="35">
@@ -2239,33 +2287,33 @@
         <v>17</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="45" t="s">
-        <v>60</v>
+      <c r="D22" s="32" t="s">
+        <v>127</v>
       </c>
       <c r="E22" s="32">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="33">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H22" s="33">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I22" s="34">
         <v>3</v>
       </c>
       <c r="J22" s="35">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K22" s="43" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="L22" s="35"/>
       <c r="M22" s="35">
@@ -2283,31 +2331,31 @@
       <c r="B23" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="E23" s="32">
-        <v>50</v>
+      <c r="D23" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="E23" s="45">
+        <v>60</v>
       </c>
       <c r="F23" s="33"/>
       <c r="G23" s="33">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H23" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" s="34">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="J23" s="35">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="K23" s="43" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="L23" s="35"/>
       <c r="M23" s="35">
@@ -2325,15 +2373,13 @@
       <c r="B24" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="E24" s="45">
-        <v>60</v>
-      </c>
+      <c r="C24" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="32"/>
       <c r="F24" s="33"/>
       <c r="G24" s="33">
         <v>3</v>
@@ -2342,14 +2388,14 @@
         <v>1</v>
       </c>
       <c r="I24" s="34">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="J24" s="35">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="K24" s="43" t="s">
-        <v>133</v>
+        <v>55</v>
       </c>
       <c r="L24" s="35"/>
       <c r="M24" s="35">
@@ -2367,29 +2413,31 @@
       <c r="B25" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="32"/>
+      <c r="C25" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>93</v>
+      </c>
       <c r="F25" s="33"/>
       <c r="G25" s="33">
-        <v>3</v>
+        <v>1225</v>
       </c>
       <c r="H25" s="33">
-        <v>1</v>
+        <v>1225</v>
       </c>
       <c r="I25" s="34">
-        <v>3</v>
+        <v>0.08</v>
       </c>
       <c r="J25" s="35">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="K25" s="43" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="L25" s="35"/>
       <c r="M25" s="35">
@@ -2408,30 +2456,30 @@
         <v>131</v>
       </c>
       <c r="C26" s="45" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D26" s="45" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>93</v>
+        <v>106</v>
+      </c>
+      <c r="E26" s="45">
+        <v>30</v>
       </c>
       <c r="F26" s="33"/>
       <c r="G26" s="33">
-        <v>1225</v>
+        <v>3</v>
       </c>
       <c r="H26" s="33">
-        <v>1225</v>
+        <v>2</v>
       </c>
       <c r="I26" s="34">
-        <v>0.08</v>
+        <v>2.5</v>
       </c>
       <c r="J26" s="35">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="K26" s="43" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="L26" s="35"/>
       <c r="M26" s="35">
@@ -2444,37 +2492,30 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="B27" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="45">
-        <v>30</v>
+      <c r="C27" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="32">
+        <v>20</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="33">
         <v>3</v>
       </c>
       <c r="H27" s="33">
-        <v>2</v>
-      </c>
-      <c r="I27" s="34">
-        <v>2.5</v>
-      </c>
-      <c r="J27" s="35">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="K27" s="43" t="s">
-        <v>107</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I27" s="34"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="43"/>
       <c r="L27" s="35"/>
       <c r="M27" s="35">
         <f t="shared" si="1"/>
@@ -2488,28 +2529,29 @@
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="45" t="s">
-        <v>131</v>
-      </c>
+      <c r="B28" s="32"/>
       <c r="C28" s="32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="32">
-        <v>20</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="E28" s="32"/>
       <c r="F28" s="33"/>
       <c r="G28" s="33">
-        <v>3</v>
+        <v>76</v>
       </c>
       <c r="H28" s="33">
-        <v>3</v>
-      </c>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="43"/>
+        <v>100</v>
+      </c>
+      <c r="I28" s="34">
+        <v>0.11</v>
+      </c>
+      <c r="J28" s="35">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="K28" s="3"/>
       <c r="L28" s="35"/>
       <c r="M28" s="35">
         <f t="shared" si="1"/>
@@ -2525,25 +2567,25 @@
       </c>
       <c r="B29" s="32"/>
       <c r="C29" s="32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="33"/>
       <c r="G29" s="33">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="H29" s="33">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I29" s="34">
-        <v>0.11</v>
+        <v>0.3</v>
       </c>
       <c r="J29" s="35">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="35"/>
@@ -2561,25 +2603,25 @@
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="H30" s="33">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I30" s="34">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="J30" s="35">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="35"/>
@@ -2597,10 +2639,10 @@
       </c>
       <c r="B31" s="32"/>
       <c r="C31" s="32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="33"/>
@@ -2611,11 +2653,11 @@
         <v>100</v>
       </c>
       <c r="I31" s="34">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
       <c r="J31" s="35">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="35"/>
@@ -2625,35 +2667,41 @@
       </c>
       <c r="N31" s="35"/>
       <c r="O31" s="32"/>
-      <c r="P31" s="3"/>
+      <c r="P31" s="3">
+        <v>7380</v>
+      </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32" t="s">
+      <c r="B32" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="D32" s="32" t="s">
-        <v>59</v>
+      <c r="D32" s="45" t="s">
+        <v>134</v>
       </c>
       <c r="E32" s="32"/>
       <c r="F32" s="33"/>
       <c r="G32" s="33">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="H32" s="33">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="I32" s="34">
-        <v>0.21</v>
+        <v>4</v>
       </c>
       <c r="J32" s="35">
         <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="K32" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="K32" s="43" t="s">
+        <v>135</v>
+      </c>
       <c r="L32" s="35"/>
       <c r="M32" s="35">
         <f t="shared" si="1"/>
@@ -2661,9 +2709,7 @@
       </c>
       <c r="N32" s="35"/>
       <c r="O32" s="32"/>
-      <c r="P32" s="3">
-        <v>7380</v>
-      </c>
+      <c r="P32" s="3"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -3541,8 +3587,8 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="39">
-        <f>SUM(J16:J51)</f>
-        <v>756.46</v>
+        <f>SUM(J15:J51)</f>
+        <v>768.46</v>
       </c>
       <c r="K57" s="44"/>
       <c r="L57" s="39"/>
@@ -3552,7 +3598,7 @@
       <c r="P57" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A11:P55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A10:P55" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:P2"/>
@@ -3565,31 +3611,32 @@
     <hyperlink ref="K49" r:id="rId5" display="Link" xr:uid="{B9C35A18-9E24-41B8-8C22-68FEA326621C}"/>
     <hyperlink ref="N50" r:id="rId6" display="Compact Powerful Motor" xr:uid="{9EFF2727-C3AB-4597-8B26-0F812CAFC429}"/>
     <hyperlink ref="N51" r:id="rId7" xr:uid="{605BE8D7-BA93-4401-9D46-9E08E1D04442}"/>
-    <hyperlink ref="K21" r:id="rId8" display="Link" xr:uid="{695B4940-C0A7-4809-BDF2-0C233AA6AE26}"/>
-    <hyperlink ref="K23" r:id="rId9" display="2x Length: 45mm 4PC" xr:uid="{6B68950A-869F-4FCE-BC1C-F219E055C5B9}"/>
+    <hyperlink ref="K20" r:id="rId8" display="Link" xr:uid="{695B4940-C0A7-4809-BDF2-0C233AA6AE26}"/>
+    <hyperlink ref="K22" r:id="rId9" display="2x Length: 45mm 4PC" xr:uid="{6B68950A-869F-4FCE-BC1C-F219E055C5B9}"/>
     <hyperlink ref="K33" r:id="rId10" xr:uid="{24787D90-0D34-481E-9743-F212E75A3881}"/>
-    <hyperlink ref="K25" r:id="rId11" xr:uid="{D6A1DF84-384D-40FB-BD4A-701A0F364D79}"/>
+    <hyperlink ref="K24" r:id="rId11" xr:uid="{D6A1DF84-384D-40FB-BD4A-701A0F364D79}"/>
     <hyperlink ref="N46" r:id="rId12" display="Gates" xr:uid="{E093F5B4-8BAD-4356-A43B-07E9B513EAC3}"/>
     <hyperlink ref="N47" r:id="rId13" display="Gates" xr:uid="{49D5B23E-126C-4370-A262-C5184F11CAFE}"/>
     <hyperlink ref="N48" r:id="rId14" display="Pulley 20 Tooth 9mm" xr:uid="{27F936CE-C292-435B-B7DE-316A6986F2BD}"/>
-    <hyperlink ref="K26" r:id="rId15" xr:uid="{A8C5E0F3-B1FB-4E57-8DD8-1DF57CDC1A28}"/>
+    <hyperlink ref="K25" r:id="rId15" xr:uid="{A8C5E0F3-B1FB-4E57-8DD8-1DF57CDC1A28}"/>
     <hyperlink ref="K35" r:id="rId16" xr:uid="{ACB41F0C-D739-4C4C-B9A7-3FBBB0E03C0B}"/>
     <hyperlink ref="K34" r:id="rId17" display="FYSETC Big Dipper" xr:uid="{531DCC85-6FB5-4C6C-8657-8A481CD30069}"/>
     <hyperlink ref="K36" r:id="rId18" display="6pcs Optical Endstop" xr:uid="{0AB90FFF-9946-4F78-93E2-A102C645ECAE}"/>
     <hyperlink ref="K37" r:id="rId19" xr:uid="{1A2B703D-766E-449D-AD03-BDC8990C9635}"/>
-    <hyperlink ref="K22" r:id="rId20" xr:uid="{7E1F7424-E58C-4FCB-9D3A-3CB69F34CE9F}"/>
-    <hyperlink ref="K27" r:id="rId21" xr:uid="{755FCD6D-D745-447C-AAA6-2D31A19F9A40}"/>
+    <hyperlink ref="K21" r:id="rId20" xr:uid="{7E1F7424-E58C-4FCB-9D3A-3CB69F34CE9F}"/>
+    <hyperlink ref="K26" r:id="rId21" xr:uid="{755FCD6D-D745-447C-AAA6-2D31A19F9A40}"/>
     <hyperlink ref="K41" r:id="rId22" xr:uid="{A90E869A-7328-473A-BA20-82979A845F00}"/>
     <hyperlink ref="K42" r:id="rId23" xr:uid="{37B2932B-CA7B-49AA-9F35-9BCE3D136353}"/>
     <hyperlink ref="K43" r:id="rId24" xr:uid="{BE140B59-D4B8-46C3-B6EC-BEB5F431781F}"/>
     <hyperlink ref="K44" r:id="rId25" xr:uid="{54817A0E-3A4B-42D7-AA92-5C84B2F161F2}"/>
     <hyperlink ref="K38" r:id="rId26" xr:uid="{4F053E16-31A4-458E-B422-7E74FE54E665}"/>
     <hyperlink ref="N38" r:id="rId27" display="Color: 220V 750W" xr:uid="{6A46011B-C1CA-4A88-AD58-75064F9710C4}"/>
-    <hyperlink ref="K24" r:id="rId28" xr:uid="{D81B7FCC-2A0B-49BE-B9F6-1DF3B108016A}"/>
+    <hyperlink ref="K23" r:id="rId28" xr:uid="{D81B7FCC-2A0B-49BE-B9F6-1DF3B108016A}"/>
+    <hyperlink ref="K32" r:id="rId29" xr:uid="{B9B35946-F710-4A9B-AA0F-C3E1EB8A9B02}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId29"/>
-  <drawing r:id="rId30"/>
-  <legacyDrawing r:id="rId31"/>
+  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId30"/>
+  <drawing r:id="rId31"/>
+  <legacyDrawing r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>